<commit_message>
Add location details form and individual details xls/xml and updating others forms
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/change_household_head.xlsx
+++ b/xforms/xlsforms/change_household_head.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13650" tabRatio="500"/>
+    <workbookView windowWidth="28695" windowHeight="14175" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
   <si>
     <t>type</t>
   </si>
@@ -84,7 +84,7 @@
     <t>visitId</t>
   </si>
   <si>
-    <t>Id da visita</t>
+    <t>1. ExtId da visita</t>
   </si>
   <si>
     <t>Visit Id</t>
@@ -96,7 +96,7 @@
     <t>visitDate</t>
   </si>
   <si>
-    <t>Data da visita</t>
+    <t>2. Data da visita</t>
   </si>
   <si>
     <t>VIsit Date</t>
@@ -105,7 +105,7 @@
     <t>fieldWorkerId</t>
   </si>
   <si>
-    <t>Código do Inquiridor</t>
+    <t>3. Código do Inquiridor</t>
   </si>
   <si>
     <t>Field Worker Id</t>
@@ -114,7 +114,7 @@
     <t>householdId</t>
   </si>
   <si>
-    <t>Id do Agregado</t>
+    <t>3. ExtId do Agregado</t>
   </si>
   <si>
     <t>HouseHoldId</t>
@@ -123,7 +123,7 @@
     <t>householdName</t>
   </si>
   <si>
-    <t>Número do Agregado</t>
+    <t>5. Número do Agregado</t>
   </si>
   <si>
     <t>Household Name</t>
@@ -132,7 +132,7 @@
     <t>new_hoh_id</t>
   </si>
   <si>
-    <t>Novo ID do Chefe de agregado</t>
+    <t>6. ExtId do Novo Chefe de agregado</t>
   </si>
   <si>
     <t>New Hoh Id</t>
@@ -141,7 +141,7 @@
     <t>new_hoh_name</t>
   </si>
   <si>
-    <t>Nome do novo Chefe de Agregado</t>
+    <t>7. Nome do Novo Chefe de Agregado</t>
   </si>
   <si>
     <t>New Hoh Name</t>
@@ -150,7 +150,7 @@
     <t>eventDate</t>
   </si>
   <si>
-    <t>Data da mudança</t>
+    <t>8. Data da mudança</t>
   </si>
   <si>
     <t>Date of change</t>
@@ -162,7 +162,7 @@
     <t>causes</t>
   </si>
   <si>
-    <t>Causa da mudança de chefe</t>
+    <t>9. Causa da mudança de chefe</t>
   </si>
   <si>
     <t>Cause of the change</t>
@@ -171,6 +171,9 @@
     <t>otherCauses</t>
   </si>
   <si>
+    <t>9.1. Especifique as causas da mudança</t>
+  </si>
+  <si>
     <t>Especifique as causas da mudança</t>
   </si>
   <si>
@@ -183,7 +186,7 @@
     <t>hh_people_nb</t>
   </si>
   <si>
-    <t>Membros do Agregado</t>
+    <t>10. Número de Membros do Agregado</t>
   </si>
   <si>
     <t>Members</t>
@@ -195,7 +198,7 @@
     <t>membershiptonewhoh</t>
   </si>
   <si>
-    <t>Alterar Filiação dos Membros</t>
+    <t>11. Relação dos membros com o chefe</t>
   </si>
   <si>
     <t>Membership</t>
@@ -207,7 +210,7 @@
     <t>extId</t>
   </si>
   <si>
-    <t>ExtId do Membro</t>
+    <t>1. ExtId do Membro</t>
   </si>
   <si>
     <t>Member Id</t>
@@ -216,7 +219,7 @@
     <t>memberName</t>
   </si>
   <si>
-    <t>Nome do membro</t>
+    <t>2. Nome do membro</t>
   </si>
   <si>
     <t>Member Name</t>
@@ -234,7 +237,7 @@
     <t>relationshipToGroupHead</t>
   </si>
   <si>
-    <t>Relação com o chefe de agregado</t>
+    <t>4. Relação com o chefe de agregado</t>
   </si>
   <si>
     <t>Relationship to Group Head</t>
@@ -387,7 +390,7 @@
     <t>Portuguese</t>
   </si>
   <si>
-    <t>concat("CHANGE_HOH-",${householdName})</t>
+    <t>concat("MudarChefe-",${householdName})</t>
   </si>
 </sst>
 </file>
@@ -396,9 +399,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -452,7 +455,99 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -467,39 +562,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,82 +584,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -596,6 +599,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -608,175 +617,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -805,21 +814,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -834,6 +828,36 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -855,6 +879,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -863,179 +896,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1060,6 +1069,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1077,7 +1089,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1151,10 +1163,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="221F1E"/>
+        <a:sysClr val="windowText" lastClr="141312"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="E0E9EE"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1476,537 +1488,539 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="31.0866666666667" style="13" customWidth="1"/>
-    <col min="2" max="2" width="26.6266666666667" style="13" customWidth="1"/>
-    <col min="3" max="4" width="30.1266666666667" style="13" customWidth="1"/>
-    <col min="5" max="5" width="21.5" style="13" customWidth="1"/>
-    <col min="6" max="6" width="22.8733333333333" style="13" customWidth="1"/>
-    <col min="7" max="7" width="25" style="13" customWidth="1"/>
-    <col min="8" max="8" width="10.8733333333333" style="13"/>
-    <col min="9" max="9" width="37.2533333333333" style="13" customWidth="1"/>
-    <col min="10" max="10" width="10.8733333333333" style="13"/>
-    <col min="11" max="11" width="19.1266666666667" style="13" customWidth="1"/>
-    <col min="12" max="16" width="10.8733333333333" style="13"/>
-    <col min="17" max="17" width="12" style="13" customWidth="1"/>
-    <col min="18" max="16384" width="10.8733333333333" style="13"/>
+    <col min="1" max="1" width="31.0866666666667" style="14" customWidth="1"/>
+    <col min="2" max="2" width="26.6266666666667" style="14" customWidth="1"/>
+    <col min="3" max="4" width="30.1266666666667" style="14" customWidth="1"/>
+    <col min="5" max="5" width="21.5" style="14" customWidth="1"/>
+    <col min="6" max="6" width="22.8733333333333" style="14" customWidth="1"/>
+    <col min="7" max="7" width="25" style="14" customWidth="1"/>
+    <col min="8" max="8" width="10.8733333333333" style="14"/>
+    <col min="9" max="9" width="37.2533333333333" style="14" customWidth="1"/>
+    <col min="10" max="10" width="10.8733333333333" style="14"/>
+    <col min="11" max="11" width="19.1266666666667" style="14" customWidth="1"/>
+    <col min="12" max="16" width="10.8733333333333" style="14"/>
+    <col min="17" max="17" width="12" style="14" customWidth="1"/>
+    <col min="18" max="16384" width="10.8733333333333" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
     </row>
     <row r="5" ht="17.25" customHeight="1" spans="1:12">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="13" t="b">
+      <c r="H5" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1" spans="1:12">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="13" t="b">
+      <c r="H6" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="13" t="b">
+      <c r="H7" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="L8" s="13" t="b">
+      <c r="H8" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="L9" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" ht="11" customHeight="1" spans="1:12">
-      <c r="A10" s="13" t="s">
+      <c r="H9" s="15"/>
+      <c r="L9" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:12">
+      <c r="A10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="L10" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" ht="11" customHeight="1" spans="1:12">
-      <c r="A11" s="13" t="s">
+      <c r="H10" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="23" customHeight="1" spans="1:12">
+      <c r="A11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="L11" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="13" t="s">
+      <c r="H11" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="23" customHeight="1" spans="1:8">
+      <c r="A12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="16" t="s">
+      <c r="H12" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="17" customHeight="1" spans="1:8">
+      <c r="A13" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="16" t="s">
+      <c r="H13" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" ht="19" customHeight="1" spans="1:9">
+      <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="21" t="s">
+      <c r="D14" s="17" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" ht="13.5" customHeight="1" spans="1:12">
-      <c r="A15" s="13" t="s">
+      <c r="H14" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="13" t="s">
+    </row>
+    <row r="15" ht="18" customHeight="1" spans="1:12">
+      <c r="A15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="C15" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="13" t="b">
+      <c r="D15" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="13" t="s">
+      <c r="L15" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" ht="14" customHeight="1" spans="1:17">
+      <c r="A16" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="Q16" s="13" t="s">
+      <c r="D16" s="14" t="s">
         <v>61</v>
       </c>
+      <c r="Q16" s="14" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="H17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="L17" s="13" t="b">
+      <c r="D17" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="H17" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="C18" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="H18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="L18" s="13" t="b">
+      <c r="D18" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="H18" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="19" t="s">
+      <c r="B19" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="H19" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="L19" s="13" t="b">
+      <c r="D19" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="H19" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" spans="1:8">
-      <c r="A20" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="B20" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="C20" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="H20" s="13" t="b">
+      <c r="D20" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="H20" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="A21" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="L22" s="13" t="b">
+      <c r="A22" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L22" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="8:8">
-      <c r="H23" s="20"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="31" spans="8:8">
-      <c r="H31" s="20"/>
+      <c r="H31" s="21"/>
     </row>
     <row r="32" spans="8:8">
-      <c r="H32" s="20"/>
+      <c r="H32" s="21"/>
     </row>
     <row r="33" spans="8:8">
-      <c r="H33" s="20"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="8:8">
-      <c r="H34" s="20"/>
+      <c r="H34" s="21"/>
     </row>
     <row r="35" spans="8:8">
-      <c r="H35" s="20"/>
+      <c r="H35" s="21"/>
     </row>
     <row r="52" spans="8:8">
-      <c r="H52" s="20"/>
+      <c r="H52" s="21"/>
     </row>
     <row r="53" spans="8:8">
-      <c r="H53" s="20"/>
+      <c r="H53" s="21"/>
     </row>
     <row r="54" spans="8:8">
-      <c r="H54" s="20"/>
+      <c r="H54" s="21"/>
     </row>
     <row r="55" spans="8:8">
-      <c r="H55" s="20"/>
+      <c r="H55" s="21"/>
     </row>
     <row r="56" spans="8:8">
-      <c r="H56" s="20"/>
+      <c r="H56" s="21"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="20"/>
-      <c r="H57" s="20"/>
+      <c r="A57" s="21"/>
+      <c r="H57" s="21"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="20"/>
-      <c r="H58" s="20"/>
+      <c r="A58" s="21"/>
+      <c r="H58" s="21"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="20"/>
-      <c r="H59" s="20"/>
+      <c r="A59" s="21"/>
+      <c r="H59" s="21"/>
     </row>
     <row r="60" spans="8:8">
-      <c r="H60" s="20"/>
+      <c r="H60" s="21"/>
     </row>
     <row r="62" spans="8:8">
-      <c r="H62" s="20"/>
+      <c r="H62" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2020,15 +2034,15 @@
   <sheetPr/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8733333333333" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="30.2533333333333" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.3" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.1266666666667" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.3" style="4" customWidth="1"/>
     <col min="4" max="4" width="24.1" style="4" customWidth="1"/>
     <col min="5" max="5" width="18.7533333333333" style="4" customWidth="1"/>
     <col min="6" max="16384" width="10.8733333333333" style="4"/>
@@ -2036,7 +2050,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -2045,7 +2059,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -2053,313 +2067,313 @@
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B2" s="8">
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="8">
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" ht="18" customHeight="1" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="8">
         <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" ht="18" customHeight="1" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" s="8">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" s="8">
         <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="8">
         <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1" spans="1:5">
       <c r="A8" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B8" s="8">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="8">
-        <v>9</v>
+        <v>72</v>
+      </c>
+      <c r="B9" s="10">
+        <v>88</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" ht="14.25" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>105</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" ht="14.25" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="10">
+        <v>103</v>
+      </c>
+      <c r="B11" s="11">
         <v>2</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>108</v>
       </c>
+      <c r="E11" s="12" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="12" ht="14.25" spans="1:5">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="10">
-        <v>1</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>109</v>
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="13" ht="14.25" spans="1:5">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="11">
         <v>2</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>110</v>
+      <c r="C13" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" ht="14.25" spans="1:5">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="11">
         <v>3</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>111</v>
+      <c r="C14" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="15" ht="14.25" spans="1:5">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="11">
         <v>4</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>112</v>
+      <c r="C15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" ht="14.25" spans="1:5">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="11">
         <v>5</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>113</v>
+      <c r="C16" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" ht="14.25" spans="1:5">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="11">
         <v>6</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>114</v>
+      <c r="C17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="18" ht="14.25" spans="1:5">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="11">
         <v>99</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>115</v>
+      <c r="C18" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" ht="14.25" spans="1:5">
-      <c r="A19" s="12"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" ht="14.25" spans="1:5">
-      <c r="A20" s="12"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" ht="14.25" spans="1:5">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="11"/>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" ht="14.25" spans="2:4">
       <c r="B22" s="8"/>
@@ -2422,35 +2436,35 @@
     <col min="1" max="1" width="37.8" customWidth="1"/>
     <col min="2" max="2" width="22.3" customWidth="1"/>
     <col min="3" max="3" width="15.2533333333333" customWidth="1"/>
-    <col min="4" max="4" width="29.7533333333333" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>